<commit_message>
Code and Folder updates
</commit_message>
<xml_diff>
--- a/Professional_Development_Plan_2025/Professional Skills Matrix.xlsx
+++ b/Professional_Development_Plan_2025/Professional Skills Matrix.xlsx
@@ -5,16 +5,20 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/natalinikolic/Desktop/EssexPG/MODULE 3/e-portfolio/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/natalinikolic/Desktop/EssexPG/MODULE 3/e-portfolio/Professional_Development_Plan_2025/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D95AD259-F25E-B245-911C-ADC0BFB0D157}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7156D493-2482-AE4F-9E26-5874708F4AD0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="33480" windowHeight="24200" xr2:uid="{F0AC6F20-2752-4433-AA8C-078D6A73E621}"/>
+    <workbookView xWindow="1620" yWindow="920" windowWidth="33480" windowHeight="24200" xr2:uid="{F0AC6F20-2752-4433-AA8C-078D6A73E621}"/>
   </bookViews>
   <sheets>
     <sheet name="Skills Matrix" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Sheet1!$A$1:$C$12</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -33,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="80">
   <si>
     <t>Competency</t>
   </si>
@@ -449,7 +453,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -495,50 +499,41 @@
       <alignment horizontal="left" vertical="center" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -857,7 +852,7 @@
   <dimension ref="A1:I42"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="138" zoomScaleNormal="138" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -887,16 +882,16 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="30" t="s">
+      <c r="H1" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="30"/>
+      <c r="I1" s="25"/>
     </row>
     <row r="2" spans="1:9" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="27" t="s">
+      <c r="A2" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="22" t="s">
+      <c r="B2" s="23" t="s">
         <v>7</v>
       </c>
       <c r="C2" s="3" t="s">
@@ -916,8 +911,8 @@
       </c>
     </row>
     <row r="3" spans="1:9" s="2" customFormat="1" ht="33" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="27"/>
-      <c r="B3" s="23"/>
+      <c r="A3" s="20"/>
+      <c r="B3" s="24"/>
       <c r="C3" s="5" t="s">
         <v>11</v>
       </c>
@@ -935,8 +930,8 @@
       </c>
     </row>
     <row r="4" spans="1:9" s="2" customFormat="1" ht="49" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="27"/>
-      <c r="B4" s="21" t="s">
+      <c r="A4" s="20"/>
+      <c r="B4" s="22" t="s">
         <v>14</v>
       </c>
       <c r="C4" s="3" t="s">
@@ -956,8 +951,8 @@
       </c>
     </row>
     <row r="5" spans="1:9" s="2" customFormat="1" ht="48" x14ac:dyDescent="0.2">
-      <c r="A5" s="27"/>
-      <c r="B5" s="22"/>
+      <c r="A5" s="20"/>
+      <c r="B5" s="23"/>
       <c r="C5" s="7" t="s">
         <v>65</v>
       </c>
@@ -975,8 +970,8 @@
       </c>
     </row>
     <row r="6" spans="1:9" s="2" customFormat="1" ht="32" x14ac:dyDescent="0.2">
-      <c r="A6" s="27"/>
-      <c r="B6" s="22"/>
+      <c r="A6" s="20"/>
+      <c r="B6" s="23"/>
       <c r="C6" s="7" t="s">
         <v>20</v>
       </c>
@@ -988,8 +983,8 @@
       </c>
     </row>
     <row r="7" spans="1:9" s="2" customFormat="1" ht="32" x14ac:dyDescent="0.2">
-      <c r="A7" s="27"/>
-      <c r="B7" s="22"/>
+      <c r="A7" s="20"/>
+      <c r="B7" s="23"/>
       <c r="C7" s="7" t="s">
         <v>21</v>
       </c>
@@ -1001,8 +996,8 @@
       </c>
     </row>
     <row r="8" spans="1:9" s="2" customFormat="1" ht="33" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="27"/>
-      <c r="B8" s="23"/>
+      <c r="A8" s="20"/>
+      <c r="B8" s="24"/>
       <c r="C8" s="5" t="s">
         <v>22</v>
       </c>
@@ -1014,8 +1009,8 @@
       </c>
     </row>
     <row r="9" spans="1:9" ht="48" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="27"/>
-      <c r="B9" s="21" t="s">
+      <c r="A9" s="20"/>
+      <c r="B9" s="22" t="s">
         <v>23</v>
       </c>
       <c r="C9" s="3" t="s">
@@ -1024,41 +1019,41 @@
       <c r="D9" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="E9" s="31" t="s">
+      <c r="E9" s="3" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="53" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="27"/>
-      <c r="B10" s="22"/>
+      <c r="A10" s="20"/>
+      <c r="B10" s="23"/>
       <c r="C10" s="7" t="s">
         <v>25</v>
       </c>
       <c r="D10" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="E10" s="32" t="s">
+      <c r="E10" s="7" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="36.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="27"/>
-      <c r="B11" s="23"/>
+      <c r="A11" s="20"/>
+      <c r="B11" s="24"/>
       <c r="C11" s="5" t="s">
         <v>26</v>
       </c>
       <c r="D11" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="E11" s="33" t="s">
+      <c r="E11" s="5" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="12" spans="1:9" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="19" t="s">
+      <c r="A12" s="26" t="s">
         <v>27</v>
       </c>
-      <c r="B12" s="21" t="s">
+      <c r="B12" s="22" t="s">
         <v>28</v>
       </c>
       <c r="C12" s="3" t="s">
@@ -1070,8 +1065,8 @@
       <c r="E12" s="3"/>
     </row>
     <row r="13" spans="1:9" s="2" customFormat="1" ht="33" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="20"/>
-      <c r="B13" s="22"/>
+      <c r="A13" s="27"/>
+      <c r="B13" s="23"/>
       <c r="C13" s="7" t="s">
         <v>30</v>
       </c>
@@ -1081,7 +1076,7 @@
       <c r="E13" s="7"/>
     </row>
     <row r="14" spans="1:9" s="2" customFormat="1" ht="33" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="19" t="s">
+      <c r="A14" s="26" t="s">
         <v>31</v>
       </c>
       <c r="B14" s="6" t="s">
@@ -1096,8 +1091,8 @@
       <c r="E14" s="3"/>
     </row>
     <row r="15" spans="1:9" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="20"/>
-      <c r="B15" s="21" t="s">
+      <c r="A15" s="27"/>
+      <c r="B15" s="22" t="s">
         <v>34</v>
       </c>
       <c r="C15" s="3" t="s">
@@ -1111,8 +1106,8 @@
       </c>
     </row>
     <row r="16" spans="1:9" s="2" customFormat="1" ht="32" x14ac:dyDescent="0.2">
-      <c r="A16" s="20"/>
-      <c r="B16" s="22"/>
+      <c r="A16" s="27"/>
+      <c r="B16" s="23"/>
       <c r="C16" s="7" t="s">
         <v>36</v>
       </c>
@@ -1124,8 +1119,8 @@
       </c>
     </row>
     <row r="17" spans="1:5" s="2" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A17" s="20"/>
-      <c r="B17" s="22"/>
+      <c r="A17" s="27"/>
+      <c r="B17" s="23"/>
       <c r="C17" s="7" t="s">
         <v>37</v>
       </c>
@@ -1137,8 +1132,8 @@
       </c>
     </row>
     <row r="18" spans="1:5" s="2" customFormat="1" ht="38" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="20"/>
-      <c r="B18" s="23"/>
+      <c r="A18" s="27"/>
+      <c r="B18" s="24"/>
       <c r="C18" s="7" t="s">
         <v>38</v>
       </c>
@@ -1150,8 +1145,8 @@
       </c>
     </row>
     <row r="19" spans="1:5" s="2" customFormat="1" ht="46" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="20"/>
-      <c r="B19" s="24" t="s">
+      <c r="A19" s="27"/>
+      <c r="B19" s="28" t="s">
         <v>39</v>
       </c>
       <c r="C19" s="3" t="s">
@@ -1163,8 +1158,8 @@
       <c r="E19" s="3"/>
     </row>
     <row r="20" spans="1:5" s="2" customFormat="1" ht="49" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="20"/>
-      <c r="B20" s="25"/>
+      <c r="A20" s="27"/>
+      <c r="B20" s="29"/>
       <c r="C20" s="5" t="s">
         <v>41</v>
       </c>
@@ -1176,10 +1171,10 @@
       </c>
     </row>
     <row r="21" spans="1:5" s="2" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="26" t="s">
+      <c r="A21" s="19" t="s">
         <v>42</v>
       </c>
-      <c r="B21" s="24" t="s">
+      <c r="B21" s="28" t="s">
         <v>43</v>
       </c>
       <c r="C21" s="13" t="s">
@@ -1189,52 +1184,50 @@
       <c r="E21" s="7"/>
     </row>
     <row r="22" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A22" s="27"/>
-      <c r="B22" s="28"/>
+      <c r="A22" s="20"/>
+      <c r="B22" s="30"/>
       <c r="C22" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="D22" s="12" t="s">
-        <v>9</v>
-      </c>
+      <c r="D22" s="12"/>
       <c r="E22" s="14"/>
     </row>
     <row r="23" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A23" s="27"/>
-      <c r="B23" s="28"/>
+      <c r="A23" s="20"/>
+      <c r="B23" s="30"/>
       <c r="C23" s="7" t="s">
         <v>46</v>
       </c>
       <c r="D23" s="12" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="E23" s="14"/>
     </row>
     <row r="24" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A24" s="27"/>
-      <c r="B24" s="28"/>
+      <c r="A24" s="20"/>
+      <c r="B24" s="30"/>
       <c r="C24" s="15" t="s">
         <v>77</v>
       </c>
       <c r="D24" s="12" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="E24" s="14"/>
     </row>
     <row r="25" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A25" s="27"/>
-      <c r="B25" s="28"/>
+      <c r="A25" s="20"/>
+      <c r="B25" s="30"/>
       <c r="C25" s="15" t="s">
         <v>76</v>
       </c>
       <c r="D25" s="12" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="E25" s="14"/>
     </row>
     <row r="26" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A26" s="27"/>
-      <c r="B26" s="28"/>
+      <c r="A26" s="20"/>
+      <c r="B26" s="30"/>
       <c r="C26" s="15" t="s">
         <v>47</v>
       </c>
@@ -1244,19 +1237,19 @@
       <c r="E26" s="14"/>
     </row>
     <row r="27" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A27" s="27"/>
-      <c r="B27" s="28"/>
+      <c r="A27" s="20"/>
+      <c r="B27" s="30"/>
       <c r="C27" s="7" t="s">
         <v>48</v>
       </c>
       <c r="D27" s="12" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="E27" s="14"/>
     </row>
     <row r="28" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A28" s="27"/>
-      <c r="B28" s="28"/>
+      <c r="A28" s="20"/>
+      <c r="B28" s="30"/>
       <c r="C28" s="7" t="s">
         <v>49</v>
       </c>
@@ -1266,8 +1259,8 @@
       <c r="E28" s="14"/>
     </row>
     <row r="29" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A29" s="27"/>
-      <c r="B29" s="28"/>
+      <c r="A29" s="20"/>
+      <c r="B29" s="30"/>
       <c r="C29" s="7" t="s">
         <v>50</v>
       </c>
@@ -1277,8 +1270,8 @@
       <c r="E29" s="14"/>
     </row>
     <row r="30" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A30" s="27"/>
-      <c r="B30" s="28"/>
+      <c r="A30" s="20"/>
+      <c r="B30" s="30"/>
       <c r="C30" s="7" t="s">
         <v>51</v>
       </c>
@@ -1288,19 +1281,19 @@
       <c r="E30" s="14"/>
     </row>
     <row r="31" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A31" s="27"/>
-      <c r="B31" s="28"/>
+      <c r="A31" s="20"/>
+      <c r="B31" s="30"/>
       <c r="C31" s="7" t="s">
         <v>52</v>
       </c>
       <c r="D31" s="12" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E31" s="14"/>
     </row>
     <row r="32" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="27"/>
-      <c r="B32" s="28"/>
+      <c r="A32" s="20"/>
+      <c r="B32" s="30"/>
       <c r="C32" s="5" t="s">
         <v>53</v>
       </c>
@@ -1310,10 +1303,10 @@
       <c r="E32" s="14"/>
     </row>
     <row r="33" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A33" s="26" t="s">
+      <c r="A33" s="19" t="s">
         <v>54</v>
       </c>
-      <c r="B33" s="21" t="s">
+      <c r="B33" s="22" t="s">
         <v>55</v>
       </c>
       <c r="C33" s="3" t="s">
@@ -1325,8 +1318,8 @@
       <c r="E33" s="8"/>
     </row>
     <row r="34" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A34" s="27"/>
-      <c r="B34" s="22"/>
+      <c r="A34" s="20"/>
+      <c r="B34" s="23"/>
       <c r="C34" s="7" t="s">
         <v>57</v>
       </c>
@@ -1336,8 +1329,8 @@
       <c r="E34" s="9"/>
     </row>
     <row r="35" spans="1:5" ht="33" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="27"/>
-      <c r="B35" s="23"/>
+      <c r="A35" s="20"/>
+      <c r="B35" s="24"/>
       <c r="C35" s="5" t="s">
         <v>58</v>
       </c>
@@ -1347,7 +1340,7 @@
       <c r="E35" s="10"/>
     </row>
     <row r="36" spans="1:5" ht="65" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="29"/>
+      <c r="A36" s="21"/>
       <c r="B36" s="16" t="s">
         <v>59</v>
       </c>
@@ -1410,4 +1403,137 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A910D272-3489-8641-A5C2-6CCF66D44F90}">
+  <dimension ref="A1:C12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="42.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="28" t="s">
+        <v>43</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A2" s="30"/>
+      <c r="B2" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="C2" s="12"/>
+    </row>
+    <row r="3" spans="1:3" ht="48" x14ac:dyDescent="0.2">
+      <c r="A3" s="30"/>
+      <c r="B3" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A4" s="30"/>
+      <c r="B4" s="15" t="s">
+        <v>77</v>
+      </c>
+      <c r="C4" s="12" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="32" x14ac:dyDescent="0.2">
+      <c r="A5" s="30"/>
+      <c r="B5" s="15" t="s">
+        <v>76</v>
+      </c>
+      <c r="C5" s="12" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A6" s="30"/>
+      <c r="B6" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="C6" s="12"/>
+    </row>
+    <row r="7" spans="1:3" ht="48" x14ac:dyDescent="0.2">
+      <c r="A7" s="30"/>
+      <c r="B7" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="C7" s="12" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="32" x14ac:dyDescent="0.2">
+      <c r="A8" s="30"/>
+      <c r="B8" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="C8" s="12" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="96" x14ac:dyDescent="0.2">
+      <c r="A9" s="30"/>
+      <c r="B9" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="C9" s="12" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="96" x14ac:dyDescent="0.2">
+      <c r="A10" s="30"/>
+      <c r="B10" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="C10" s="12" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="80" x14ac:dyDescent="0.2">
+      <c r="A11" s="30"/>
+      <c r="B11" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="C11" s="12" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="49" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="30"/>
+      <c r="B12" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="C12" s="12" t="s">
+        <v>18</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:C12" xr:uid="{A910D272-3489-8641-A5C2-6CCF66D44F90}"/>
+  <mergeCells count="1">
+    <mergeCell ref="A1:A12"/>
+  </mergeCells>
+  <dataValidations count="1">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="C2:C12" xr:uid="{799A711C-857C-F14B-ADF4-3BB3A644D281}">
+      <formula1>$H$2:$H$5</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>